<commit_message>
feat: add all xlsx
</commit_message>
<xml_diff>
--- a/backend/src/shared/infra/typeorm/seeds/xlsx/seed_estado.xlsx
+++ b/backend/src/shared/infra/typeorm/seeds/xlsx/seed_estado.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maia/Documents/Projetos/gcm/backend/src/shared/infra/typeorm/seeds/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6EB8C48-29AE-4FC6-8BC6-B3CF8ECC24BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDB6A09-0FAD-A54F-9BD7-C2D27000B3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="460" windowWidth="27320" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="520" windowWidth="27320" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -292,11 +292,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,9 +336,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,406 +646,408 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="97" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="1"/>
+    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="1"/>
+    <col min="4" max="4" width="80.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>51</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>11</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>42</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>17</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>